<commit_message>
bug fix for linux
</commit_message>
<xml_diff>
--- a/examples/pysero_analysis_config.xlsx
+++ b/examples/pysero_analysis_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/ELISAarrayReader/images_scienion/OJ_plate3_9_7_8_4_10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE4DF69-561D-704A-95D8-DACD014EADFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0926794D-14E1-1244-A0FE-41B4F9AF1549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18980" xr2:uid="{2C8FFFCF-2234-4E43-9609-0711918053F4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18980" activeTab="5" xr2:uid="{2C8FFFCF-2234-4E43-9609-0711918053F4}"/>
   </bookViews>
   <sheets>
     <sheet name="pysero output dirs" sheetId="1" r:id="rId1"/>
@@ -310,10 +310,10 @@
     <t># well action: If 'keep' or 'drop', the wells specified in 'well ID' column will be kept or dropped. All wells will be kept if # # NA or left empty.</t>
   </si>
   <si>
-    <t>Pool</t>
-  </si>
-  <si>
     <t>property to split the data by and plot separately. See pysero spot fitting metadata (\examples\pysero_output_data_metadata.xlsx) for available properties.</t>
+  </si>
+  <si>
+    <t>Pool,mab, CR3022</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BF5E64-59EB-464E-9E50-4B72F7790285}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="222" workbookViewId="0">
+    <sheetView zoomScale="144" zoomScaleNormal="222" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1249,7 +1249,7 @@
         <v>62</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1352,7 +1352,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="172" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1426,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C52FC3E-3CCB-654B-B043-7A418B5EADC2}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1453,7 +1453,7 @@
         <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>78</v>
@@ -1486,7 +1486,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>83</v>

</xml_diff>